<commit_message>
lly forecasts, seems overvalued
</commit_message>
<xml_diff>
--- a/SIGA.xlsx
+++ b/SIGA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425A33FB-C171-43C2-9FE7-DEB6774F744B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E604C94-E82E-4558-8CCE-70E96CBA222F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8160" yWindow="3885" windowWidth="20730" windowHeight="11475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="705" windowWidth="15405" windowHeight="15495" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="706">
   <si>
     <t>Name</t>
   </si>
@@ -2228,9 +2228,6 @@
     <t>Cases</t>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>Epi-date</t>
   </si>
   <si>
@@ -2238,6 +2235,12 @@
   </si>
   <si>
     <t>7 day MA</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
   </si>
 </sst>
 </file>
@@ -2464,7 +2467,7 @@
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2660,12 +2663,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4970,10 +4977,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30E3C55D-9118-482B-8720-4989D85F03BD}">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4981,1535 +4988,2133 @@
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="103" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="102" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="C2" s="102">
+    <row r="2" spans="1:10">
+      <c r="C2" s="101">
         <v>44770</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="101">
+        <v>44775</v>
+      </c>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" t="s">
+        <v>701</v>
+      </c>
+      <c r="H2" t="s">
+        <v>700</v>
+      </c>
+      <c r="I2" t="s">
         <v>702</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" s="105" t="s">
+        <v>704</v>
+      </c>
+      <c r="C4" s="106">
+        <f>SUM(C5:C83)</f>
+        <v>21148</v>
+      </c>
+      <c r="D4" s="106">
+        <f>SUM(D5:D82)</f>
+        <v>23618</v>
+      </c>
+      <c r="E4" s="107">
+        <f>+D4/C4-1</f>
+        <v>0.11679591450728211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="B5" t="s">
+        <v>699</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f>+D5-C5</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="101">
+        <v>44698</v>
+      </c>
+      <c r="H5" s="103">
+        <v>1</v>
+      </c>
+      <c r="I5" s="103">
+        <f>+H5</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="103"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="B6" t="s">
+        <v>698</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E70" si="0">+D6-C6</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="101">
+        <v>44701</v>
+      </c>
+      <c r="H6" s="103">
+        <v>1</v>
+      </c>
+      <c r="I6" s="103">
+        <f>+H6+I5</f>
+        <v>2</v>
+      </c>
+      <c r="J6" s="103"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="B7" t="s">
+        <v>697</v>
+      </c>
+      <c r="C7">
+        <v>44</v>
+      </c>
+      <c r="D7">
+        <v>45</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="101">
+        <v>44702</v>
+      </c>
+      <c r="H7" s="103">
+        <v>2</v>
+      </c>
+      <c r="I7" s="103">
+        <f t="shared" ref="I7:I69" si="1">+H7+I6</f>
+        <v>4</v>
+      </c>
+      <c r="J7" s="103"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" t="s">
+        <v>696</v>
+      </c>
+      <c r="C8">
+        <v>118</v>
+      </c>
+      <c r="D8">
+        <v>132</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G8" s="101">
+        <v>44704</v>
+      </c>
+      <c r="H8" s="103">
+        <v>2</v>
+      </c>
+      <c r="I8" s="103">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J8" s="103"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="B9" t="s">
+        <v>695</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="101">
+        <v>44705</v>
+      </c>
+      <c r="H9" s="103">
+        <v>2</v>
+      </c>
+      <c r="I9" s="103">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J9" s="103"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" t="s">
+        <v>694</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="101">
+        <v>44706</v>
+      </c>
+      <c r="H10" s="103">
+        <v>2</v>
+      </c>
+      <c r="I10" s="103">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J10" s="103"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" t="s">
+        <v>693</v>
+      </c>
+      <c r="C11">
+        <v>393</v>
+      </c>
+      <c r="D11">
+        <v>393</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="101">
+        <v>44707</v>
+      </c>
+      <c r="H11" s="103">
+        <v>2</v>
+      </c>
+      <c r="I11" s="103">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J11" s="103">
+        <f>SUM(H5:H11)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" t="s">
+        <v>692</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="101">
+        <v>44708</v>
+      </c>
+      <c r="H12" s="103">
+        <v>1</v>
+      </c>
+      <c r="I12" s="103">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J12" s="103">
+        <f t="shared" ref="J12:J69" si="2">SUM(H6:H12)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" t="s">
+        <v>691</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="101">
+        <v>44710</v>
+      </c>
+      <c r="H13" s="103">
+        <v>2</v>
+      </c>
+      <c r="I13" s="103">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J13" s="103">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" t="s">
+        <v>690</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="101">
+        <v>44712</v>
+      </c>
+      <c r="H14" s="103">
+        <v>3</v>
+      </c>
+      <c r="I14" s="103">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J14" s="103">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" t="s">
+        <v>689</v>
+      </c>
+      <c r="C15">
+        <v>696</v>
+      </c>
+      <c r="D15">
+        <v>978</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>282</v>
+      </c>
+      <c r="G15" s="101">
+        <v>44713</v>
+      </c>
+      <c r="H15" s="103">
+        <v>1</v>
+      </c>
+      <c r="I15" s="103">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J15" s="103">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" t="s">
+        <v>688</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="101">
+        <v>44714</v>
+      </c>
+      <c r="H16" s="103">
+        <v>3</v>
+      </c>
+      <c r="I16" s="103">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="J16" s="103">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" t="s">
+        <v>687</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="101">
+        <v>44715</v>
+      </c>
+      <c r="H17" s="103">
+        <v>4</v>
+      </c>
+      <c r="I17" s="103">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="J17" s="103">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" t="s">
+        <v>686</v>
+      </c>
+      <c r="C18">
+        <v>745</v>
+      </c>
+      <c r="D18">
+        <v>803</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="G18" s="101">
+        <v>44716</v>
+      </c>
+      <c r="H18" s="103">
+        <v>1</v>
+      </c>
+      <c r="I18" s="103">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="J18" s="103">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" t="s">
+        <v>685</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="101">
+        <v>44718</v>
+      </c>
+      <c r="H19" s="103">
+        <v>6</v>
+      </c>
+      <c r="I19" s="103">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J19" s="103">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" t="s">
+        <v>684</v>
+      </c>
+      <c r="C20">
+        <v>45</v>
+      </c>
+      <c r="D20">
+        <v>55</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G20" s="101">
+        <v>44719</v>
+      </c>
+      <c r="H20" s="103">
+        <v>2</v>
+      </c>
+      <c r="I20" s="103">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="J20" s="103">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" t="s">
+        <v>683</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="101">
+        <v>44720</v>
+      </c>
+      <c r="H21" s="103">
+        <v>5</v>
+      </c>
+      <c r="I21" s="103">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J21" s="103">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" t="s">
+        <v>682</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="101">
+        <v>44721</v>
+      </c>
+      <c r="H22" s="103">
+        <v>2</v>
+      </c>
+      <c r="I22" s="103">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="J22" s="103">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C23">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G23" s="101">
+        <v>44722</v>
+      </c>
+      <c r="H23" s="103">
+        <v>4</v>
+      </c>
+      <c r="I23" s="103">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="J23" s="103">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" t="s">
+        <v>680</v>
+      </c>
+      <c r="C24">
+        <v>19</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G24" s="101">
+        <v>44723</v>
+      </c>
+      <c r="H24" s="103">
+        <v>4</v>
+      </c>
+      <c r="I24" s="103">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J24" s="103">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" t="s">
+        <v>679</v>
+      </c>
+      <c r="C25">
+        <v>163</v>
+      </c>
+      <c r="D25">
+        <v>163</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="101">
+        <v>44724</v>
+      </c>
+      <c r="H25" s="103">
+        <v>2</v>
+      </c>
+      <c r="I25" s="103">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="J25" s="103">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" t="s">
+        <v>678</v>
+      </c>
+      <c r="C26">
+        <v>76</v>
+      </c>
+      <c r="D26">
+        <v>99</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="G26" s="101">
+        <v>44725</v>
+      </c>
+      <c r="H26" s="103">
+        <v>2</v>
+      </c>
+      <c r="I26" s="103">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="J26" s="103">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" t="s">
+        <v>677</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="101">
+        <v>44726</v>
+      </c>
+      <c r="H27" s="103">
+        <v>11</v>
+      </c>
+      <c r="I27" s="103">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="J27" s="103">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" t="s">
+        <v>676</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="101">
+        <v>44727</v>
+      </c>
+      <c r="H28" s="103">
+        <v>7</v>
+      </c>
+      <c r="I28" s="103">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="J28" s="103">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" t="s">
+        <v>675</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G29" s="101">
+        <v>44728</v>
+      </c>
+      <c r="H29" s="103">
+        <v>13</v>
+      </c>
+      <c r="I29" s="103">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="J29" s="103">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" t="s">
+        <v>674</v>
+      </c>
+      <c r="C30">
+        <v>17</v>
+      </c>
+      <c r="D30">
+        <v>17</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="101">
+        <v>44729</v>
+      </c>
+      <c r="H30" s="103">
+        <v>4</v>
+      </c>
+      <c r="I30" s="103">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="J30" s="103">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" t="s">
+        <v>673</v>
+      </c>
+      <c r="C31">
+        <v>1837</v>
+      </c>
+      <c r="D31">
+        <v>1955</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="G31" s="101">
+        <v>44730</v>
+      </c>
+      <c r="H31" s="103">
+        <v>11</v>
+      </c>
+      <c r="I31" s="103">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="J31" s="103">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" t="s">
+        <v>672</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="101">
+        <v>44731</v>
+      </c>
+      <c r="H32" s="103">
+        <v>5</v>
+      </c>
+      <c r="I32" s="103">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="J32" s="103">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" t="s">
+        <v>671</v>
+      </c>
+      <c r="C33">
+        <v>2540</v>
+      </c>
+      <c r="D33">
+        <v>2677</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>137</v>
+      </c>
+      <c r="G33" s="101">
+        <v>44732</v>
+      </c>
+      <c r="H33" s="103">
+        <v>7</v>
+      </c>
+      <c r="I33" s="103">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="J33" s="103">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" t="s">
+        <v>670</v>
+      </c>
+      <c r="C34">
+        <v>30</v>
+      </c>
+      <c r="D34">
+        <v>30</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="101">
+        <v>44733</v>
+      </c>
+      <c r="H34" s="103">
+        <v>15</v>
+      </c>
+      <c r="I34" s="103">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="J34" s="103">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" t="s">
+        <v>669</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="101">
+        <v>44734</v>
+      </c>
+      <c r="H35" s="103">
+        <v>19</v>
+      </c>
+      <c r="I35" s="103">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+      <c r="J35" s="103">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" t="s">
+        <v>668</v>
+      </c>
+      <c r="C36">
+        <v>32</v>
+      </c>
+      <c r="D36">
+        <v>32</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="101">
+        <v>44735</v>
+      </c>
+      <c r="H36" s="103">
+        <v>19</v>
+      </c>
+      <c r="I36" s="103">
+        <f t="shared" si="1"/>
+        <v>165</v>
+      </c>
+      <c r="J36" s="103">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" t="s">
+        <v>667</v>
+      </c>
+      <c r="C37">
+        <v>37</v>
+      </c>
+      <c r="D37">
+        <v>39</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G37" s="101">
+        <v>44736</v>
+      </c>
+      <c r="H37" s="103">
+        <v>35</v>
+      </c>
+      <c r="I37" s="103">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="J37" s="103">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" t="s">
+        <v>666</v>
+      </c>
+      <c r="C38">
+        <v>9</v>
+      </c>
+      <c r="D38">
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G38" s="101">
+        <v>44737</v>
+      </c>
+      <c r="H38" s="103">
+        <v>12</v>
+      </c>
+      <c r="I38" s="103">
+        <f t="shared" si="1"/>
+        <v>212</v>
+      </c>
+      <c r="J38" s="103">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" t="s">
+        <v>665</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G39" s="101">
+        <v>44738</v>
+      </c>
+      <c r="H39" s="103">
+        <v>12</v>
+      </c>
+      <c r="I39" s="103">
+        <f t="shared" si="1"/>
+        <v>224</v>
+      </c>
+      <c r="J39" s="103">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" t="s">
+        <v>664</v>
+      </c>
+      <c r="C40">
+        <v>85</v>
+      </c>
+      <c r="D40">
+        <v>85</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G40" s="101">
+        <v>44739</v>
+      </c>
+      <c r="H40" s="103">
+        <v>53</v>
+      </c>
+      <c r="I40" s="103">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+      <c r="J40" s="103">
+        <f t="shared" si="2"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" t="s">
+        <v>663</v>
+      </c>
+      <c r="C41">
+        <v>133</v>
+      </c>
+      <c r="D41">
+        <v>146</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G41" s="101">
+        <v>44740</v>
+      </c>
+      <c r="H41" s="103">
+        <v>30</v>
+      </c>
+      <c r="I41" s="103">
+        <f t="shared" si="1"/>
+        <v>307</v>
+      </c>
+      <c r="J41" s="103">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" t="s">
+        <v>662</v>
+      </c>
+      <c r="C42">
+        <v>426</v>
+      </c>
+      <c r="D42">
+        <v>479</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="G42" s="101">
+        <v>44741</v>
+      </c>
+      <c r="H42" s="103">
+        <v>42</v>
+      </c>
+      <c r="I42" s="103">
+        <f t="shared" si="1"/>
+        <v>349</v>
+      </c>
+      <c r="J42" s="103">
+        <f t="shared" si="2"/>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="B43" t="s">
+        <v>661</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G43" s="101">
+        <v>44742</v>
+      </c>
+      <c r="H43" s="103">
+        <v>57</v>
+      </c>
+      <c r="I43" s="103">
+        <f t="shared" si="1"/>
+        <v>406</v>
+      </c>
+      <c r="J43" s="103">
+        <f t="shared" si="2"/>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="B44" t="s">
+        <v>660</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G44" s="101">
+        <v>44743</v>
+      </c>
+      <c r="H44" s="103">
+        <v>52</v>
+      </c>
+      <c r="I44" s="103">
+        <f t="shared" si="1"/>
+        <v>458</v>
+      </c>
+      <c r="J44" s="103">
+        <f t="shared" si="2"/>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="B45" t="s">
+        <v>659</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G45" s="101">
+        <v>44744</v>
+      </c>
+      <c r="H45" s="103">
+        <v>16</v>
+      </c>
+      <c r="I45" s="103">
+        <f t="shared" si="1"/>
+        <v>474</v>
+      </c>
+      <c r="J45" s="103">
+        <f t="shared" si="2"/>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="B46" t="s">
+        <v>658</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G46" s="101">
+        <v>44745</v>
+      </c>
+      <c r="H46" s="103">
+        <v>11</v>
+      </c>
+      <c r="I46" s="103">
+        <f t="shared" si="1"/>
+        <v>485</v>
+      </c>
+      <c r="J46" s="103">
+        <f t="shared" si="2"/>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="B47" t="s">
+        <v>657</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G47" s="101">
+        <v>44746</v>
+      </c>
+      <c r="H47" s="103">
+        <v>7</v>
+      </c>
+      <c r="I47" s="103">
+        <f t="shared" si="1"/>
+        <v>492</v>
+      </c>
+      <c r="J47" s="103">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="B48" t="s">
+        <v>656</v>
+      </c>
+      <c r="C48">
+        <v>23</v>
+      </c>
+      <c r="D48">
+        <v>30</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G48" s="101">
+        <v>44747</v>
+      </c>
+      <c r="H48" s="103">
+        <v>37</v>
+      </c>
+      <c r="I48" s="103">
+        <f t="shared" si="1"/>
+        <v>529</v>
+      </c>
+      <c r="J48" s="103">
+        <f t="shared" si="2"/>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="B49" t="s">
+        <v>655</v>
+      </c>
+      <c r="C49">
+        <v>17</v>
+      </c>
+      <c r="D49">
+        <v>17</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G49" s="101">
+        <v>44748</v>
+      </c>
+      <c r="H49" s="103">
+        <v>45</v>
+      </c>
+      <c r="I49" s="103">
+        <f t="shared" si="1"/>
+        <v>574</v>
+      </c>
+      <c r="J49" s="103">
+        <f t="shared" si="2"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="B50" t="s">
+        <v>654</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G50" s="101">
+        <v>44749</v>
+      </c>
+      <c r="H50" s="103">
+        <v>52</v>
+      </c>
+      <c r="I50" s="103">
+        <f t="shared" si="1"/>
+        <v>626</v>
+      </c>
+      <c r="J50" s="103">
+        <f t="shared" si="2"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="B51" t="s">
+        <v>653</v>
+      </c>
+      <c r="C51">
+        <v>59</v>
+      </c>
+      <c r="D51">
+        <v>59</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G51" s="101">
+        <v>44750</v>
+      </c>
+      <c r="H51" s="103">
+        <v>37</v>
+      </c>
+      <c r="I51" s="103">
+        <f t="shared" si="1"/>
+        <v>663</v>
+      </c>
+      <c r="J51" s="103">
+        <f t="shared" si="2"/>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="B52" t="s">
+        <v>652</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G52" s="101">
+        <v>44751</v>
+      </c>
+      <c r="H52" s="103">
+        <v>37</v>
+      </c>
+      <c r="I52" s="103">
+        <f t="shared" si="1"/>
         <v>700</v>
       </c>
-      <c r="G2" t="s">
-        <v>703</v>
-      </c>
-      <c r="H2" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="B3" t="s">
-        <v>701</v>
-      </c>
-      <c r="C3" t="s">
-        <v>700</v>
-      </c>
-      <c r="E3" s="102">
-        <v>44698</v>
-      </c>
-      <c r="F3" s="104">
+      <c r="J52" s="103">
+        <f t="shared" si="2"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="B53" t="s">
+        <v>651</v>
+      </c>
+      <c r="C53">
+        <v>878</v>
+      </c>
+      <c r="D53">
+        <v>925</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="G53" s="101">
+        <v>44752</v>
+      </c>
+      <c r="H53" s="103">
+        <v>7</v>
+      </c>
+      <c r="I53" s="103">
+        <f t="shared" si="1"/>
+        <v>707</v>
+      </c>
+      <c r="J53" s="103">
+        <f t="shared" si="2"/>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="B54" t="s">
+        <v>650</v>
+      </c>
+      <c r="C54">
         <v>1</v>
       </c>
-      <c r="G3" s="104">
-        <f>+F3</f>
+      <c r="D54">
         <v>1</v>
       </c>
-      <c r="H3" s="104"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="B4" t="s">
-        <v>699</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="E4" s="102">
-        <v>44701</v>
-      </c>
-      <c r="F4" s="104">
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G54" s="101">
+        <v>44753</v>
+      </c>
+      <c r="H54" s="103">
+        <v>100</v>
+      </c>
+      <c r="I54" s="103">
+        <f t="shared" si="1"/>
+        <v>807</v>
+      </c>
+      <c r="J54" s="103">
+        <f t="shared" si="2"/>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" t="s">
+        <v>649</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G55" s="101">
+        <v>44754</v>
+      </c>
+      <c r="H55" s="103">
+        <v>212</v>
+      </c>
+      <c r="I55" s="103">
+        <f t="shared" si="1"/>
+        <v>1019</v>
+      </c>
+      <c r="J55" s="103">
+        <f t="shared" si="2"/>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" t="s">
+        <v>648</v>
+      </c>
+      <c r="C56">
+        <v>133</v>
+      </c>
+      <c r="D56">
+        <v>133</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G56" s="101">
+        <v>44755</v>
+      </c>
+      <c r="H56" s="103">
+        <v>140</v>
+      </c>
+      <c r="I56" s="103">
+        <f t="shared" si="1"/>
+        <v>1159</v>
+      </c>
+      <c r="J56" s="103">
+        <f t="shared" si="2"/>
+        <v>585</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10">
+      <c r="B57" t="s">
+        <v>647</v>
+      </c>
+      <c r="C57">
+        <v>51</v>
+      </c>
+      <c r="D57">
+        <v>55</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G57" s="101">
+        <v>44756</v>
+      </c>
+      <c r="H57" s="103">
+        <v>216</v>
+      </c>
+      <c r="I57" s="103">
+        <f t="shared" si="1"/>
+        <v>1375</v>
+      </c>
+      <c r="J57" s="103">
+        <f t="shared" si="2"/>
+        <v>749</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="B58" t="s">
+        <v>646</v>
+      </c>
+      <c r="C58">
         <v>1</v>
       </c>
-      <c r="G4" s="104">
-        <f>+F4+G3</f>
-        <v>2</v>
-      </c>
-      <c r="H4" s="104"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="B5" t="s">
-        <v>698</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-      <c r="E5" s="102">
-        <v>44702</v>
-      </c>
-      <c r="F5" s="104">
-        <v>2</v>
-      </c>
-      <c r="G5" s="104">
-        <f t="shared" ref="G5:G66" si="0">+F5+G4</f>
-        <v>4</v>
-      </c>
-      <c r="H5" s="104"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="B6" t="s">
-        <v>697</v>
-      </c>
-      <c r="C6">
-        <v>44</v>
-      </c>
-      <c r="E6" s="102">
-        <v>44704</v>
-      </c>
-      <c r="F6" s="104">
-        <v>2</v>
-      </c>
-      <c r="G6" s="104">
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G58" s="101">
+        <v>44757</v>
+      </c>
+      <c r="H58" s="103">
+        <v>159</v>
+      </c>
+      <c r="I58" s="103">
+        <f t="shared" si="1"/>
+        <v>1534</v>
+      </c>
+      <c r="J58" s="103">
+        <f t="shared" si="2"/>
+        <v>871</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10">
+      <c r="B59" t="s">
+        <v>645</v>
+      </c>
+      <c r="C59">
+        <v>251</v>
+      </c>
+      <c r="D59">
+        <v>305</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="G59" s="101">
+        <v>44758</v>
+      </c>
+      <c r="H59" s="103">
+        <v>7</v>
+      </c>
+      <c r="I59" s="103">
+        <f t="shared" si="1"/>
+        <v>1541</v>
+      </c>
+      <c r="J59" s="103">
+        <f t="shared" si="2"/>
+        <v>841</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10">
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G60" s="101"/>
+      <c r="H60" s="103"/>
+      <c r="I60" s="103"/>
+      <c r="J60" s="103"/>
+    </row>
+    <row r="61" spans="2:10">
+      <c r="B61" t="s">
+        <v>644</v>
+      </c>
+      <c r="C61">
+        <v>53</v>
+      </c>
+      <c r="D61">
+        <v>59</v>
+      </c>
+      <c r="E61">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H6" s="104"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7" t="s">
-        <v>696</v>
-      </c>
-      <c r="C7">
-        <v>118</v>
-      </c>
-      <c r="E7" s="102">
-        <v>44705</v>
-      </c>
-      <c r="F7" s="104">
+      <c r="G61" s="101">
+        <v>44759</v>
+      </c>
+      <c r="H61" s="103">
+        <v>1</v>
+      </c>
+      <c r="I61" s="103">
+        <f>+H61+I59</f>
+        <v>1542</v>
+      </c>
+      <c r="J61" s="103">
+        <f>SUM(H54:H61)</f>
+        <v>835</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10">
+      <c r="B62" t="s">
+        <v>643</v>
+      </c>
+      <c r="C62">
+        <v>588</v>
+      </c>
+      <c r="D62">
+        <v>633</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="G62" s="101">
+        <v>44760</v>
+      </c>
+      <c r="H62" s="103">
+        <v>195</v>
+      </c>
+      <c r="I62" s="103">
+        <f t="shared" si="1"/>
+        <v>1737</v>
+      </c>
+      <c r="J62" s="103">
+        <f>SUM(H55:H62)</f>
+        <v>930</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10">
+      <c r="B63" t="s">
+        <v>642</v>
+      </c>
+      <c r="C63">
         <v>2</v>
       </c>
-      <c r="G7" s="104">
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H7" s="104"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8" t="s">
-        <v>695</v>
-      </c>
-      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="G63" s="101">
+        <v>44761</v>
+      </c>
+      <c r="H63" s="103">
+        <v>301</v>
+      </c>
+      <c r="I63" s="103">
+        <f t="shared" si="1"/>
+        <v>2038</v>
+      </c>
+      <c r="J63" s="103">
+        <f>SUM(H56:H63)</f>
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10">
+      <c r="B64" t="s">
+        <v>641</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G64" s="101">
+        <v>44762</v>
+      </c>
+      <c r="H64" s="103">
+        <v>256</v>
+      </c>
+      <c r="I64" s="103">
+        <f t="shared" si="1"/>
+        <v>2294</v>
+      </c>
+      <c r="J64" s="103">
+        <f>SUM(H57:H64)</f>
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10">
+      <c r="B65" t="s">
+        <v>640</v>
+      </c>
+      <c r="C65">
+        <v>20</v>
+      </c>
+      <c r="D65">
+        <v>21</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E8" s="102">
-        <v>44706</v>
-      </c>
-      <c r="F8" s="104">
+      <c r="G65" s="101">
+        <v>44763</v>
+      </c>
+      <c r="H65" s="103">
+        <v>184</v>
+      </c>
+      <c r="I65" s="103">
+        <f t="shared" si="1"/>
+        <v>2478</v>
+      </c>
+      <c r="J65" s="103">
+        <f>SUM(H58:H65)</f>
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10">
+      <c r="B66" t="s">
+        <v>639</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G66" s="101">
+        <v>44764</v>
+      </c>
+      <c r="H66" s="103">
+        <v>308</v>
+      </c>
+      <c r="I66" s="103">
+        <f t="shared" si="1"/>
+        <v>2786</v>
+      </c>
+      <c r="J66" s="103">
+        <f>SUM(H59:H66)</f>
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10">
+      <c r="B67" t="s">
+        <v>638</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G67" s="101">
+        <v>44765</v>
+      </c>
+      <c r="H67" s="103">
+        <v>9</v>
+      </c>
+      <c r="I67" s="103">
+        <f t="shared" si="1"/>
+        <v>2795</v>
+      </c>
+      <c r="J67" s="103">
+        <f t="shared" si="2"/>
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10">
+      <c r="B68" t="s">
+        <v>637</v>
+      </c>
+      <c r="C68">
+        <v>10</v>
+      </c>
+      <c r="D68">
+        <v>10</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G68" s="101">
+        <v>44766</v>
+      </c>
+      <c r="H68" s="103">
         <v>2</v>
       </c>
-      <c r="G8" s="104">
+      <c r="I68" s="103">
+        <f t="shared" si="1"/>
+        <v>2797</v>
+      </c>
+      <c r="J68" s="103">
+        <f t="shared" si="2"/>
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10">
+      <c r="B69" t="s">
+        <v>636</v>
+      </c>
+      <c r="C69">
+        <v>11</v>
+      </c>
+      <c r="D69">
+        <v>11</v>
+      </c>
+      <c r="E69">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H8" s="104"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9" t="s">
-        <v>694</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="102">
-        <v>44707</v>
-      </c>
-      <c r="F9" s="104">
-        <v>2</v>
-      </c>
-      <c r="G9" s="104">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="H9" s="104">
-        <f>SUM(F3:F9)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="B10" t="s">
-        <v>693</v>
-      </c>
-      <c r="C10">
-        <v>393</v>
-      </c>
-      <c r="E10" s="102">
-        <v>44708</v>
-      </c>
-      <c r="F10" s="104">
-        <v>1</v>
-      </c>
-      <c r="G10" s="104">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="H10" s="104">
-        <f t="shared" ref="H10:H66" si="1">SUM(F4:F10)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="B11" t="s">
-        <v>692</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="E11" s="102">
-        <v>44710</v>
-      </c>
-      <c r="F11" s="104">
-        <v>2</v>
-      </c>
-      <c r="G11" s="104">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="H11" s="104">
+        <v>0</v>
+      </c>
+      <c r="G69" s="101">
+        <v>44767</v>
+      </c>
+      <c r="H69" s="103">
+        <v>439</v>
+      </c>
+      <c r="I69" s="103">
         <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="B12" t="s">
-        <v>691</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="102">
-        <v>44712</v>
-      </c>
-      <c r="F12" s="104">
-        <v>3</v>
-      </c>
-      <c r="G12" s="104">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="H12" s="104">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="B13" t="s">
-        <v>690</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="102">
-        <v>44713</v>
-      </c>
-      <c r="F13" s="104">
-        <v>1</v>
-      </c>
-      <c r="G13" s="104">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="H13" s="104">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="B14" t="s">
-        <v>689</v>
-      </c>
-      <c r="C14">
-        <v>696</v>
-      </c>
-      <c r="E14" s="102">
-        <v>44714</v>
-      </c>
-      <c r="F14" s="104">
-        <v>3</v>
-      </c>
-      <c r="G14" s="104">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="H14" s="104">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="B15" t="s">
-        <v>688</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="E15" s="102">
-        <v>44715</v>
-      </c>
-      <c r="F15" s="104">
-        <v>4</v>
-      </c>
-      <c r="G15" s="104">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="H15" s="104">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="B16" t="s">
-        <v>687</v>
-      </c>
-      <c r="C16">
-        <v>7</v>
-      </c>
-      <c r="E16" s="102">
-        <v>44716</v>
-      </c>
-      <c r="F16" s="104">
-        <v>1</v>
-      </c>
-      <c r="G16" s="104">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="H16" s="104">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" t="s">
-        <v>686</v>
-      </c>
-      <c r="C17">
-        <v>745</v>
-      </c>
-      <c r="E17" s="102">
-        <v>44718</v>
-      </c>
-      <c r="F17" s="104">
-        <v>6</v>
-      </c>
-      <c r="G17" s="104">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="H17" s="104">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" t="s">
-        <v>685</v>
-      </c>
-      <c r="C18">
-        <v>8</v>
-      </c>
-      <c r="E18" s="102">
-        <v>44719</v>
-      </c>
-      <c r="F18" s="104">
-        <v>2</v>
-      </c>
-      <c r="G18" s="104">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="H18" s="104">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" t="s">
-        <v>684</v>
-      </c>
-      <c r="C19">
-        <v>45</v>
-      </c>
-      <c r="E19" s="102">
-        <v>44720</v>
-      </c>
-      <c r="F19" s="104">
-        <v>5</v>
-      </c>
-      <c r="G19" s="104">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="H19" s="104">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" t="s">
-        <v>683</v>
-      </c>
-      <c r="C20">
-        <v>12</v>
-      </c>
-      <c r="E20" s="102">
-        <v>44721</v>
-      </c>
-      <c r="F20" s="104">
-        <v>2</v>
-      </c>
-      <c r="G20" s="104">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="H20" s="104">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" t="s">
-        <v>682</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="E21" s="102">
-        <v>44722</v>
-      </c>
-      <c r="F21" s="104">
-        <v>4</v>
-      </c>
-      <c r="G21" s="104">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="H21" s="104">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" t="s">
-        <v>681</v>
-      </c>
-      <c r="C22">
-        <v>11</v>
-      </c>
-      <c r="E22" s="102">
-        <v>44723</v>
-      </c>
-      <c r="F22" s="104">
-        <v>4</v>
-      </c>
-      <c r="G22" s="104">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="H22" s="104">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" t="s">
-        <v>680</v>
-      </c>
-      <c r="C23">
-        <v>19</v>
-      </c>
-      <c r="E23" s="102">
-        <v>44724</v>
-      </c>
-      <c r="F23" s="104">
-        <v>2</v>
-      </c>
-      <c r="G23" s="104">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="H23" s="104">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" t="s">
-        <v>679</v>
-      </c>
-      <c r="C24">
-        <v>163</v>
-      </c>
-      <c r="E24" s="102">
-        <v>44725</v>
-      </c>
-      <c r="F24" s="104">
-        <v>2</v>
-      </c>
-      <c r="G24" s="104">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="H24" s="104">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="B25" t="s">
-        <v>678</v>
-      </c>
-      <c r="C25">
-        <v>76</v>
-      </c>
-      <c r="E25" s="102">
-        <v>44726</v>
-      </c>
-      <c r="F25" s="104">
-        <v>11</v>
-      </c>
-      <c r="G25" s="104">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="H25" s="104">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" t="s">
-        <v>677</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="E26" s="102">
-        <v>44727</v>
-      </c>
-      <c r="F26" s="104">
-        <v>7</v>
-      </c>
-      <c r="G26" s="104">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="H26" s="104">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8">
-      <c r="B27" t="s">
-        <v>676</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="E27" s="102">
-        <v>44728</v>
-      </c>
-      <c r="F27" s="104">
-        <v>13</v>
-      </c>
-      <c r="G27" s="104">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="H27" s="104">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8">
-      <c r="B28" t="s">
-        <v>675</v>
-      </c>
-      <c r="C28">
-        <v>5</v>
-      </c>
-      <c r="E28" s="102">
-        <v>44729</v>
-      </c>
-      <c r="F28" s="104">
-        <v>4</v>
-      </c>
-      <c r="G28" s="104">
-        <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
-      <c r="H28" s="104">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8">
-      <c r="B29" t="s">
-        <v>674</v>
-      </c>
-      <c r="C29">
-        <v>17</v>
-      </c>
-      <c r="E29" s="102">
-        <v>44730</v>
-      </c>
-      <c r="F29" s="104">
-        <v>11</v>
-      </c>
-      <c r="G29" s="104">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="H29" s="104">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8">
-      <c r="B30" t="s">
-        <v>673</v>
-      </c>
-      <c r="C30">
-        <v>1837</v>
-      </c>
-      <c r="E30" s="102">
-        <v>44731</v>
-      </c>
-      <c r="F30" s="104">
-        <v>5</v>
-      </c>
-      <c r="G30" s="104">
-        <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-      <c r="H30" s="104">
-        <f t="shared" si="1"/>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8">
-      <c r="B31" t="s">
-        <v>672</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="E31" s="102">
-        <v>44732</v>
-      </c>
-      <c r="F31" s="104">
-        <v>7</v>
-      </c>
-      <c r="G31" s="104">
-        <f t="shared" si="0"/>
-        <v>112</v>
-      </c>
-      <c r="H31" s="104">
-        <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8">
-      <c r="B32" t="s">
-        <v>671</v>
-      </c>
-      <c r="C32">
-        <v>2540</v>
-      </c>
-      <c r="E32" s="102">
-        <v>44733</v>
-      </c>
-      <c r="F32" s="104">
-        <v>15</v>
-      </c>
-      <c r="G32" s="104">
-        <f t="shared" si="0"/>
-        <v>127</v>
-      </c>
-      <c r="H32" s="104">
-        <f t="shared" si="1"/>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8">
-      <c r="B33" t="s">
-        <v>670</v>
-      </c>
-      <c r="C33">
-        <v>30</v>
-      </c>
-      <c r="E33" s="102">
-        <v>44734</v>
-      </c>
-      <c r="F33" s="104">
-        <v>19</v>
-      </c>
-      <c r="G33" s="104">
-        <f t="shared" si="0"/>
-        <v>146</v>
-      </c>
-      <c r="H33" s="104">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8">
-      <c r="B34" t="s">
-        <v>669</v>
-      </c>
-      <c r="C34">
-        <v>5</v>
-      </c>
-      <c r="E34" s="102">
-        <v>44735</v>
-      </c>
-      <c r="F34" s="104">
-        <v>19</v>
-      </c>
-      <c r="G34" s="104">
-        <f t="shared" si="0"/>
-        <v>165</v>
-      </c>
-      <c r="H34" s="104">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8">
-      <c r="B35" t="s">
-        <v>668</v>
-      </c>
-      <c r="C35">
-        <v>32</v>
-      </c>
-      <c r="E35" s="102">
-        <v>44736</v>
-      </c>
-      <c r="F35" s="104">
-        <v>35</v>
-      </c>
-      <c r="G35" s="104">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="H35" s="104">
-        <f t="shared" si="1"/>
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8">
-      <c r="B36" t="s">
-        <v>667</v>
-      </c>
-      <c r="C36">
-        <v>37</v>
-      </c>
-      <c r="E36" s="102">
-        <v>44737</v>
-      </c>
-      <c r="F36" s="104">
-        <v>12</v>
-      </c>
-      <c r="G36" s="104">
-        <f t="shared" si="0"/>
-        <v>212</v>
-      </c>
-      <c r="H36" s="104">
-        <f t="shared" si="1"/>
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8">
-      <c r="B37" t="s">
-        <v>666</v>
-      </c>
-      <c r="C37">
-        <v>9</v>
-      </c>
-      <c r="E37" s="102">
-        <v>44738</v>
-      </c>
-      <c r="F37" s="104">
-        <v>12</v>
-      </c>
-      <c r="G37" s="104">
-        <f t="shared" si="0"/>
-        <v>224</v>
-      </c>
-      <c r="H37" s="104">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8">
-      <c r="B38" t="s">
-        <v>665</v>
-      </c>
-      <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="E38" s="102">
-        <v>44739</v>
-      </c>
-      <c r="F38" s="104">
-        <v>53</v>
-      </c>
-      <c r="G38" s="104">
-        <f t="shared" si="0"/>
-        <v>277</v>
-      </c>
-      <c r="H38" s="104">
-        <f t="shared" si="1"/>
-        <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8">
-      <c r="B39" t="s">
-        <v>664</v>
-      </c>
-      <c r="C39">
-        <v>85</v>
-      </c>
-      <c r="E39" s="102">
-        <v>44740</v>
-      </c>
-      <c r="F39" s="104">
-        <v>30</v>
-      </c>
-      <c r="G39" s="104">
-        <f t="shared" si="0"/>
-        <v>307</v>
-      </c>
-      <c r="H39" s="104">
-        <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8">
-      <c r="B40" t="s">
-        <v>663</v>
-      </c>
-      <c r="C40">
-        <v>133</v>
-      </c>
-      <c r="E40" s="102">
-        <v>44741</v>
-      </c>
-      <c r="F40" s="104">
-        <v>42</v>
-      </c>
-      <c r="G40" s="104">
-        <f t="shared" si="0"/>
-        <v>349</v>
-      </c>
-      <c r="H40" s="104">
-        <f t="shared" si="1"/>
-        <v>203</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8">
-      <c r="B41" t="s">
-        <v>662</v>
-      </c>
-      <c r="C41">
-        <v>426</v>
-      </c>
-      <c r="E41" s="102">
-        <v>44742</v>
-      </c>
-      <c r="F41" s="104">
-        <v>57</v>
-      </c>
-      <c r="G41" s="104">
-        <f t="shared" si="0"/>
-        <v>406</v>
-      </c>
-      <c r="H41" s="104">
-        <f t="shared" si="1"/>
-        <v>241</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8">
-      <c r="B42" t="s">
-        <v>661</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="E42" s="102">
-        <v>44743</v>
-      </c>
-      <c r="F42" s="104">
-        <v>52</v>
-      </c>
-      <c r="G42" s="104">
-        <f t="shared" si="0"/>
-        <v>458</v>
-      </c>
-      <c r="H42" s="104">
-        <f t="shared" si="1"/>
-        <v>258</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8">
-      <c r="B43" t="s">
-        <v>660</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="E43" s="102">
-        <v>44744</v>
-      </c>
-      <c r="F43" s="104">
-        <v>16</v>
-      </c>
-      <c r="G43" s="104">
-        <f t="shared" si="0"/>
-        <v>474</v>
-      </c>
-      <c r="H43" s="104">
-        <f t="shared" si="1"/>
-        <v>262</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8">
-      <c r="B44" t="s">
-        <v>659</v>
-      </c>
-      <c r="C44">
-        <v>3</v>
-      </c>
-      <c r="E44" s="102">
-        <v>44745</v>
-      </c>
-      <c r="F44" s="104">
-        <v>11</v>
-      </c>
-      <c r="G44" s="104">
-        <f t="shared" si="0"/>
-        <v>485</v>
-      </c>
-      <c r="H44" s="104">
-        <f t="shared" si="1"/>
-        <v>261</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8">
-      <c r="B45" t="s">
-        <v>658</v>
-      </c>
-      <c r="C45">
-        <v>4</v>
-      </c>
-      <c r="E45" s="102">
-        <v>44746</v>
-      </c>
-      <c r="F45" s="104">
-        <v>7</v>
-      </c>
-      <c r="G45" s="104">
-        <f t="shared" si="0"/>
-        <v>492</v>
-      </c>
-      <c r="H45" s="104">
-        <f t="shared" si="1"/>
-        <v>215</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8">
-      <c r="B46" t="s">
-        <v>657</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="E46" s="102">
-        <v>44747</v>
-      </c>
-      <c r="F46" s="104">
-        <v>37</v>
-      </c>
-      <c r="G46" s="104">
-        <f t="shared" si="0"/>
-        <v>529</v>
-      </c>
-      <c r="H46" s="104">
-        <f t="shared" si="1"/>
-        <v>222</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8">
-      <c r="B47" t="s">
-        <v>656</v>
-      </c>
-      <c r="C47">
-        <v>23</v>
-      </c>
-      <c r="E47" s="102">
-        <v>44748</v>
-      </c>
-      <c r="F47" s="104">
-        <v>45</v>
-      </c>
-      <c r="G47" s="104">
-        <f t="shared" si="0"/>
-        <v>574</v>
-      </c>
-      <c r="H47" s="104">
-        <f t="shared" si="1"/>
-        <v>225</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8">
-      <c r="B48" t="s">
-        <v>655</v>
-      </c>
-      <c r="C48">
-        <v>17</v>
-      </c>
-      <c r="E48" s="102">
-        <v>44749</v>
-      </c>
-      <c r="F48" s="104">
-        <v>52</v>
-      </c>
-      <c r="G48" s="104">
-        <f t="shared" si="0"/>
-        <v>626</v>
-      </c>
-      <c r="H48" s="104">
-        <f t="shared" si="1"/>
-        <v>220</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8">
-      <c r="B49" t="s">
-        <v>654</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="E49" s="102">
-        <v>44750</v>
-      </c>
-      <c r="F49" s="104">
-        <v>37</v>
-      </c>
-      <c r="G49" s="104">
-        <f t="shared" si="0"/>
-        <v>663</v>
-      </c>
-      <c r="H49" s="104">
-        <f t="shared" si="1"/>
-        <v>205</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8">
-      <c r="B50" t="s">
-        <v>653</v>
-      </c>
-      <c r="C50">
-        <v>59</v>
-      </c>
-      <c r="E50" s="102">
-        <v>44751</v>
-      </c>
-      <c r="F50" s="104">
-        <v>37</v>
-      </c>
-      <c r="G50" s="104">
-        <f t="shared" si="0"/>
-        <v>700</v>
-      </c>
-      <c r="H50" s="104">
-        <f t="shared" si="1"/>
-        <v>226</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8">
-      <c r="B51" t="s">
-        <v>652</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="E51" s="102">
-        <v>44752</v>
-      </c>
-      <c r="F51" s="104">
-        <v>7</v>
-      </c>
-      <c r="G51" s="104">
-        <f t="shared" si="0"/>
-        <v>707</v>
-      </c>
-      <c r="H51" s="104">
-        <f t="shared" si="1"/>
-        <v>222</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8">
-      <c r="B52" t="s">
-        <v>651</v>
-      </c>
-      <c r="C52">
-        <v>878</v>
-      </c>
-      <c r="E52" s="102">
-        <v>44753</v>
-      </c>
-      <c r="F52" s="104">
-        <v>100</v>
-      </c>
-      <c r="G52" s="104">
-        <f t="shared" si="0"/>
-        <v>807</v>
-      </c>
-      <c r="H52" s="104">
-        <f t="shared" si="1"/>
-        <v>315</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8">
-      <c r="B53" t="s">
-        <v>650</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="E53" s="102">
-        <v>44754</v>
-      </c>
-      <c r="F53" s="104">
-        <v>212</v>
-      </c>
-      <c r="G53" s="104">
-        <f t="shared" si="0"/>
-        <v>1019</v>
-      </c>
-      <c r="H53" s="104">
-        <f t="shared" si="1"/>
-        <v>490</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8">
-      <c r="B54" t="s">
-        <v>649</v>
-      </c>
-      <c r="C54">
-        <v>2</v>
-      </c>
-      <c r="E54" s="102">
-        <v>44755</v>
-      </c>
-      <c r="F54" s="104">
-        <v>140</v>
-      </c>
-      <c r="G54" s="104">
-        <f t="shared" si="0"/>
-        <v>1159</v>
-      </c>
-      <c r="H54" s="104">
-        <f t="shared" si="1"/>
-        <v>585</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8">
-      <c r="B55" t="s">
-        <v>648</v>
-      </c>
-      <c r="C55">
-        <v>133</v>
-      </c>
-      <c r="E55" s="102">
-        <v>44756</v>
-      </c>
-      <c r="F55" s="104">
-        <v>216</v>
-      </c>
-      <c r="G55" s="104">
-        <f t="shared" si="0"/>
-        <v>1375</v>
-      </c>
-      <c r="H55" s="104">
-        <f t="shared" si="1"/>
-        <v>749</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8">
-      <c r="B56" t="s">
-        <v>647</v>
-      </c>
-      <c r="C56">
-        <v>51</v>
-      </c>
-      <c r="E56" s="102">
-        <v>44757</v>
-      </c>
-      <c r="F56" s="104">
-        <v>159</v>
-      </c>
-      <c r="G56" s="104">
-        <f t="shared" si="0"/>
-        <v>1534</v>
-      </c>
-      <c r="H56" s="104">
-        <f t="shared" si="1"/>
-        <v>871</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8">
-      <c r="B57" t="s">
-        <v>646</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="E57" s="102">
-        <v>44758</v>
-      </c>
-      <c r="F57" s="104">
-        <v>7</v>
-      </c>
-      <c r="G57" s="104">
-        <f t="shared" si="0"/>
-        <v>1541</v>
-      </c>
-      <c r="H57" s="104">
-        <f t="shared" si="1"/>
-        <v>841</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8">
-      <c r="B58" t="s">
-        <v>645</v>
-      </c>
-      <c r="C58">
-        <v>251</v>
-      </c>
-      <c r="E58" s="102">
-        <v>44759</v>
-      </c>
-      <c r="F58" s="104">
-        <v>1</v>
-      </c>
-      <c r="G58" s="104">
-        <f t="shared" si="0"/>
-        <v>1542</v>
-      </c>
-      <c r="H58" s="104">
-        <f t="shared" si="1"/>
-        <v>835</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8">
-      <c r="B59" t="s">
-        <v>644</v>
-      </c>
-      <c r="C59">
-        <v>53</v>
-      </c>
-      <c r="E59" s="102">
-        <v>44760</v>
-      </c>
-      <c r="F59" s="104">
-        <v>195</v>
-      </c>
-      <c r="G59" s="104">
-        <f t="shared" si="0"/>
-        <v>1737</v>
-      </c>
-      <c r="H59" s="104">
-        <f t="shared" si="1"/>
-        <v>930</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8">
-      <c r="B60" t="s">
-        <v>643</v>
-      </c>
-      <c r="C60">
-        <v>588</v>
-      </c>
-      <c r="E60" s="102">
-        <v>44761</v>
-      </c>
-      <c r="F60" s="104">
-        <v>301</v>
-      </c>
-      <c r="G60" s="104">
-        <f t="shared" si="0"/>
-        <v>2038</v>
-      </c>
-      <c r="H60" s="104">
-        <f t="shared" si="1"/>
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8">
-      <c r="B61" t="s">
-        <v>642</v>
-      </c>
-      <c r="C61">
-        <v>2</v>
-      </c>
-      <c r="E61" s="102">
-        <v>44762</v>
-      </c>
-      <c r="F61" s="104">
-        <v>256</v>
-      </c>
-      <c r="G61" s="104">
-        <f t="shared" si="0"/>
-        <v>2294</v>
-      </c>
-      <c r="H61" s="104">
-        <f t="shared" si="1"/>
-        <v>1135</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8">
-      <c r="B62" t="s">
-        <v>641</v>
-      </c>
-      <c r="C62">
-        <v>2</v>
-      </c>
-      <c r="E62" s="102">
-        <v>44763</v>
-      </c>
-      <c r="F62" s="104">
-        <v>184</v>
-      </c>
-      <c r="G62" s="104">
-        <f t="shared" si="0"/>
-        <v>2478</v>
-      </c>
-      <c r="H62" s="104">
-        <f t="shared" si="1"/>
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8">
-      <c r="B63" t="s">
-        <v>640</v>
-      </c>
-      <c r="C63">
-        <v>20</v>
-      </c>
-      <c r="E63" s="102">
-        <v>44764</v>
-      </c>
-      <c r="F63" s="104">
-        <v>308</v>
-      </c>
-      <c r="G63" s="104">
-        <f t="shared" si="0"/>
-        <v>2786</v>
-      </c>
-      <c r="H63" s="104">
-        <f t="shared" si="1"/>
-        <v>1252</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8">
-      <c r="B64" t="s">
-        <v>639</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-      <c r="E64" s="102">
-        <v>44765</v>
-      </c>
-      <c r="F64" s="104">
-        <v>9</v>
-      </c>
-      <c r="G64" s="104">
-        <f t="shared" si="0"/>
-        <v>2795</v>
-      </c>
-      <c r="H64" s="104">
-        <f t="shared" si="1"/>
-        <v>1254</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8">
-      <c r="B65" t="s">
-        <v>638</v>
-      </c>
-      <c r="C65">
-        <v>3</v>
-      </c>
-      <c r="E65" s="102">
-        <v>44766</v>
-      </c>
-      <c r="F65" s="104">
-        <v>2</v>
-      </c>
-      <c r="G65" s="104">
-        <f t="shared" si="0"/>
-        <v>2797</v>
-      </c>
-      <c r="H65" s="104">
-        <f t="shared" si="1"/>
-        <v>1255</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8">
-      <c r="B66" t="s">
-        <v>637</v>
-      </c>
-      <c r="C66">
-        <v>10</v>
-      </c>
-      <c r="E66" s="102">
-        <v>44767</v>
-      </c>
-      <c r="F66" s="104">
-        <v>439</v>
-      </c>
-      <c r="G66" s="104">
-        <f t="shared" si="0"/>
         <v>3236</v>
       </c>
-      <c r="H66" s="104">
-        <f t="shared" si="1"/>
+      <c r="J69" s="103">
+        <f t="shared" si="2"/>
         <v>1499</v>
       </c>
     </row>
-    <row r="67" spans="2:8">
-      <c r="B67" t="s">
-        <v>636</v>
-      </c>
-      <c r="C67">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8">
-      <c r="B68" t="s">
+    <row r="70" spans="2:10">
+      <c r="B70" t="s">
         <v>635</v>
-      </c>
-      <c r="C68">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8">
-      <c r="B69" t="s">
-        <v>634</v>
-      </c>
-      <c r="C69">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="70" spans="2:8">
-      <c r="B70" t="s">
-        <v>633</v>
       </c>
       <c r="C70">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="2:8">
+      <c r="D70">
+        <v>6</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10">
       <c r="B71" t="s">
+        <v>634</v>
+      </c>
+      <c r="C71">
+        <v>33</v>
+      </c>
+      <c r="D71">
+        <v>33</v>
+      </c>
+      <c r="E71">
+        <f t="shared" ref="E71:E84" si="3">+D71-C71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10">
+      <c r="B72" t="s">
+        <v>633</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10">
+      <c r="B73" t="s">
         <v>632</v>
       </c>
-      <c r="C71">
+      <c r="C73">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="2:8">
-      <c r="B72" t="s">
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10">
+      <c r="B74" t="s">
         <v>631</v>
       </c>
-      <c r="C72">
+      <c r="C74">
         <v>3738</v>
       </c>
-    </row>
-    <row r="73" spans="2:8">
-      <c r="B73" t="s">
+      <c r="D74">
+        <v>4298</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="3"/>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10">
+      <c r="B75" t="s">
         <v>630</v>
       </c>
-      <c r="C73">
+      <c r="C75">
         <v>85</v>
       </c>
-    </row>
-    <row r="74" spans="2:8">
-      <c r="B74" t="s">
+      <c r="D75">
+        <v>88</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10">
+      <c r="B76" t="s">
         <v>629</v>
       </c>
-      <c r="C74">
+      <c r="C76">
         <v>264</v>
       </c>
-    </row>
-    <row r="75" spans="2:8">
-      <c r="B75" t="s">
+      <c r="D76">
+        <v>272</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10">
+      <c r="B77" t="s">
         <v>628</v>
       </c>
-      <c r="C75">
+      <c r="C77">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="2:8">
-      <c r="B76" t="s">
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10">
+      <c r="B78" t="s">
         <v>627</v>
       </c>
-      <c r="C76">
+      <c r="C78">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="2:8">
-      <c r="B77" t="s">
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10">
+      <c r="B79" t="s">
         <v>626</v>
       </c>
-      <c r="C77">
+      <c r="C79">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="2:8">
-      <c r="B78" t="s">
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10">
+      <c r="B80" t="s">
         <v>625</v>
       </c>
-      <c r="C78">
+      <c r="C80">
         <v>16</v>
       </c>
-    </row>
-    <row r="79" spans="2:8">
-      <c r="B79" t="s">
+      <c r="D80">
+        <v>16</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6">
+      <c r="B81" t="s">
         <v>624</v>
       </c>
-      <c r="C79">
+      <c r="C81">
         <v>2432</v>
       </c>
-    </row>
-    <row r="80" spans="2:8">
-      <c r="B80" t="s">
+      <c r="D81">
+        <v>2546</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6">
+      <c r="B82" t="s">
         <v>623</v>
       </c>
-      <c r="C80">
+      <c r="C82">
         <v>4906</v>
       </c>
-    </row>
-    <row r="81" spans="2:3">
-      <c r="B81" t="s">
+      <c r="D82">
+        <v>5810</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="3"/>
+        <v>904</v>
+      </c>
+      <c r="F82" s="108">
+        <f>+D82/C82-1</f>
+        <v>0.18426416632694664</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6">
+      <c r="B83" s="105" t="s">
+        <v>705</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6">
+      <c r="B84" t="s">
         <v>622</v>
       </c>
-      <c r="C81">
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -15329,13 +15934,13 @@
     </row>
     <row r="25" spans="2:23">
       <c r="C25" s="32"/>
-      <c r="J25" s="101" t="s">
+      <c r="J25" s="104" t="s">
         <v>298</v>
       </c>
-      <c r="K25" s="101"/>
-      <c r="L25" s="101"/>
-      <c r="M25" s="101"/>
-      <c r="N25" s="101"/>
+      <c r="K25" s="104"/>
+      <c r="L25" s="104"/>
+      <c r="M25" s="104"/>
+      <c r="N25" s="104"/>
     </row>
     <row r="26" spans="2:23">
       <c r="C26" s="68" t="s">
@@ -16817,20 +17422,20 @@
     </row>
     <row r="330" spans="2:17">
       <c r="C330" s="32"/>
-      <c r="F330" s="101" t="s">
+      <c r="F330" s="104" t="s">
         <v>459</v>
       </c>
-      <c r="G330" s="101"/>
-      <c r="H330" s="101"/>
-      <c r="I330" s="101"/>
-      <c r="J330" s="101"/>
-      <c r="K330" s="101"/>
-      <c r="L330" s="101"/>
-      <c r="M330" s="101"/>
-      <c r="N330" s="101"/>
-      <c r="O330" s="101"/>
-      <c r="P330" s="101"/>
-      <c r="Q330" s="101"/>
+      <c r="G330" s="104"/>
+      <c r="H330" s="104"/>
+      <c r="I330" s="104"/>
+      <c r="J330" s="104"/>
+      <c r="K330" s="104"/>
+      <c r="L330" s="104"/>
+      <c r="M330" s="104"/>
+      <c r="N330" s="104"/>
+      <c r="O330" s="104"/>
+      <c r="P330" s="104"/>
+      <c r="Q330" s="104"/>
     </row>
     <row r="331" spans="2:17">
       <c r="C331" s="32" t="s">
@@ -17680,12 +18285,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100764A4B226BE2F34C80DFAA3D37A3CB30" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70544b0716d1f2dd0e24adda29a3d132">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -17799,6 +18398,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B8FCBE5-DC3A-4133-9A7B-7CABB6178323}">
   <ds:schemaRefs>
@@ -17808,21 +18413,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFF1E9B8-B163-4EA4-B096-E0C9303C24CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{677EA480-9029-43DF-B2CD-874C0C4FCFF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17836,4 +18426,19 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFF1E9B8-B163-4EA4-B096-E0C9303C24CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>